<commit_message>
notebook info update pt1
</commit_message>
<xml_diff>
--- a/thesis_output/bnci/stats_final.xlsx
+++ b/thesis_output/bnci/stats_final.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itznu\PycharmProjects\use-of-snn\experiments\bnci_horizon_dataset_exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itznu\PycharmProjects\use-of-snn\thesis_output\bnci\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49EEEF8-BD7B-49D2-BED8-063299CB3339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07EFBD8-61AA-426E-920E-7FF2086E11DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -201,6 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,6 +2526,12 @@
         <v>0.63829787234042556</v>
       </c>
     </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C48" s="15">
+        <f>MAX(C28:C47)</f>
+        <v>0.51781250000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>